<commit_message>
[🛠️Fix] Equipment summon fix
- 확률 백만분율로 수정
- 10레벨까지 확장 적용 (동료, 스킬도 적용)
- 레벨별 확률 밸런싱
</commit_message>
<xml_diff>
--- a/IdleGame/Assets/@Resources/Texts/ExcelTable/SummonCount.xlsx
+++ b/IdleGame/Assets/@Resources/Texts/ExcelTable/SummonCount.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\ExcelTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\TeamProject-IdleGame\IdleGame\Assets\@Resources\Texts\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2157B4C-5C9E-40B0-8A6D-EB0FF14CD7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E2C70A-F8B1-476D-898D-3519CE7E8D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipment" sheetId="1" r:id="rId1"/>
@@ -29,10 +29,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
-    <t>D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\Texts\SummonCountEquipment.json</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>needCounts : Int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -41,11 +37,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\Texts\SummonCountSkills.json</t>
+    <t>D:\Project\TeamProject-IdleGame\IdleGame\Assets\@Resources\Texts\Summon\SummonCountEquipment.json</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\Texts\SummonCountFollower.json</t>
+    <t>D:\Project\TeamProject-IdleGame\IdleGame\Assets\@Resources\Texts\Summon\SummonCountSkills.json</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D:\Project\TeamProject-IdleGame\IdleGame\Assets\@Resources\Texts\Summon\SummonCountFollower.json</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -109,8 +109,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A34EAE5F-3DD5-47C5-A3C0-F0701D582D50}" name="표1" displayName="표1" ref="A2:B10" totalsRowShown="0">
-  <autoFilter ref="A2:B10" xr:uid="{A34EAE5F-3DD5-47C5-A3C0-F0701D582D50}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A34EAE5F-3DD5-47C5-A3C0-F0701D582D50}" name="표1" displayName="표1" ref="A2:B12" totalsRowShown="0">
+  <autoFilter ref="A2:B12" xr:uid="{A34EAE5F-3DD5-47C5-A3C0-F0701D582D50}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{04536610-14B9-409C-ADC1-249AEEBE2434}" name="SummonGrade : Int"/>
     <tableColumn id="2" xr3:uid="{CE129CB8-288D-4571-92E3-8EAE405146E8}" name="needCounts : Int"/>
@@ -120,8 +120,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1710932F-F10A-4FD4-8D72-2834CCE06636}" name="표1_3" displayName="표1_3" ref="A2:B10" totalsRowShown="0">
-  <autoFilter ref="A2:B10" xr:uid="{A34EAE5F-3DD5-47C5-A3C0-F0701D582D50}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1710932F-F10A-4FD4-8D72-2834CCE06636}" name="표1_3" displayName="표1_3" ref="A2:B12" totalsRowShown="0">
+  <autoFilter ref="A2:B12" xr:uid="{A34EAE5F-3DD5-47C5-A3C0-F0701D582D50}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{891874E8-AA0B-4D41-B049-1BBB65206487}" name="SummonGrade : Int"/>
     <tableColumn id="2" xr3:uid="{B943D1B2-2E65-4484-AD92-70E7E21708C2}" name="needCounts : Int"/>
@@ -131,8 +131,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F3C8150D-D4F6-4DBD-A72C-3666370A39BB}" name="표1_34" displayName="표1_34" ref="A2:B10" totalsRowShown="0">
-  <autoFilter ref="A2:B10" xr:uid="{A34EAE5F-3DD5-47C5-A3C0-F0701D582D50}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F3C8150D-D4F6-4DBD-A72C-3666370A39BB}" name="표1_34" displayName="표1_34" ref="A2:B12" totalsRowShown="0">
+  <autoFilter ref="A2:B12" xr:uid="{A34EAE5F-3DD5-47C5-A3C0-F0701D582D50}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{ACE059DD-63CA-4840-9E34-13481C9BBAB3}" name="SummonGrade : Int"/>
     <tableColumn id="2" xr3:uid="{B66D52E2-6239-40D1-A1D7-4B536947A029}" name="needCounts : Int"/>
@@ -404,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -418,15 +418,15 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -457,7 +457,7 @@
         <v>400</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D10" si="0">B5-B4</f>
+        <f t="shared" ref="D5:D12" si="0">B5-B4</f>
         <v>250</v>
       </c>
     </row>
@@ -519,6 +519,30 @@
       <c r="D10">
         <f t="shared" si="0"/>
         <v>2500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>12000</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>18000</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>6000</v>
       </c>
     </row>
   </sheetData>
@@ -533,7 +557,160 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED73E084-DD1B-4E57-80DF-FE69BA93276E}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="18.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>150</v>
+      </c>
+      <c r="D4">
+        <f>B4-B3</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>400</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D12" si="0">B5-B4</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2000</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>3500</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>5500</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>8000</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>12000</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>18000</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B049D74-AEDF-4727-8084-A8E8FDDD65F9}">
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -547,15 +724,15 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -586,7 +763,7 @@
         <v>400</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D10" si="0">B5-B4</f>
+        <f t="shared" ref="D5:D12" si="0">B5-B4</f>
         <v>250</v>
       </c>
     </row>
@@ -650,133 +827,28 @@
         <v>2500</v>
       </c>
     </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B049D74-AEDF-4727-8084-A8E8FDDD65F9}">
-  <dimension ref="A1:D10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="18.75" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>150</v>
-      </c>
-      <c r="D4">
-        <f>B4-B3</f>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>400</v>
-      </c>
-      <c r="D5">
-        <f t="shared" ref="D5:D10" si="0">B5-B4</f>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>1000</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>2000</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>3500</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>5500</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>8000</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>2500</v>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>12000</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>18000</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>6000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>